<commit_message>
Examples for .NET v18.10
</commit_message>
<xml_diff>
--- a/Examples/Data/02_OutputDirectory/outSourseSampleCountryNames.xlsx
+++ b/Examples/Data/02_OutputDirectory/outSourseSampleCountryNames.xlsx
@@ -564,22 +564,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15">
+    <row r="2" spans="1:1" ht="15" hidden="1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15">
+    <row r="3" spans="1:1" ht="15" hidden="1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15">
+    <row r="4" spans="1:1" ht="15" hidden="1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15">
+    <row r="5" spans="1:1" ht="15" hidden="1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -604,47 +604,47 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15">
+    <row r="10" spans="1:1" ht="15" hidden="1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15">
+    <row r="11" spans="1:1" ht="15" hidden="1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15">
+    <row r="12" spans="1:1" ht="15" hidden="1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15">
+    <row r="13" spans="1:1" ht="15" hidden="1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15">
+    <row r="14" spans="1:1" ht="15" hidden="1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15">
+    <row r="15" spans="1:1" ht="15" hidden="1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15">
+    <row r="16" spans="1:1" ht="15" hidden="1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15">
+    <row r="17" spans="1:1" ht="15" hidden="1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15">
+    <row r="18" spans="1:1" ht="15" hidden="1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -653,7 +653,7 @@
   <autoFilter ref="A1:A18">
     <filterColumn colId="0">
       <customFilters>
-        <customFilter operator="notEqual" val="*Be*"/>
+        <customFilter val="ia*"/>
       </customFilters>
     </filterColumn>
   </autoFilter>

</xml_diff>